<commit_message>
finished tp1 + start tp2
</commit_message>
<xml_diff>
--- a/TP1-A21/data_resultat.xlsx
+++ b/TP1-A21/data_resultat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanis\Desktop\Poly\A2021\INF8775\TPs\TP1-A21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF53F4DF-E04C-4A1C-872A-D32A83706C7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20110385-B355-41F4-AF39-B4ADA456A232}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D10583DE-7CAB-4211-8E9D-E4F57287116E}"/>
   </bookViews>
@@ -314,7 +314,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -992,7 +991,7 @@
                   <a:rPr lang="en-CA" sz="1000" b="0" i="0" baseline="30000">
                     <a:effectLst/>
                   </a:rPr>
-                  <a:t>3</a:t>
+                  <a:t>2.807</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-CA" sz="1000">
                   <a:effectLst/>
@@ -1470,7 +1469,7 @@
               </a:p>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000"/>
+                  <a:defRPr/>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-CA" sz="1000" b="0" i="0" baseline="0">
@@ -1482,7 +1481,7 @@
                   <a:rPr lang="en-CA" sz="1000" b="0" i="0" baseline="30000">
                     <a:effectLst/>
                   </a:rPr>
-                  <a:t>2.80</a:t>
+                  <a:t>3</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-CA" sz="1000">
                   <a:effectLst/>
@@ -2449,7 +2448,7 @@
                   <a:rPr lang="en-CA" sz="1000" b="0" i="0" baseline="30000">
                     <a:effectLst/>
                   </a:rPr>
-                  <a:t>2.80</a:t>
+                  <a:t>2.807</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-CA" sz="1000" b="0" i="0" baseline="0">
@@ -8177,16 +8176,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>337457</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>192677</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>27214</xdr:rowOff>
+      <xdr:rowOff>42454</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>489857</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>179614</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>261257</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>11974</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8213,16 +8212,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>141514</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>179614</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>232954</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>42454</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>146957</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>9797</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8585,8 +8584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D0C2ED4-B490-4C28-B94A-00AAA31F2B2B}">
   <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8720,27 +8719,27 @@
         <v>-0.29509912844475394</v>
       </c>
       <c r="U2">
-        <f>K2^3</f>
+        <f t="shared" ref="U2:U7" si="0">K2^3</f>
         <v>512</v>
       </c>
       <c r="V2">
-        <f>L2/U2</f>
+        <f t="shared" ref="V2:V7" si="1">L2/U2</f>
         <v>3.1069335937512402E-4</v>
       </c>
       <c r="W2">
-        <f>K2^2.8</f>
+        <f t="shared" ref="W2:W7" si="2">K2^2.8</f>
         <v>337.79402515786057</v>
       </c>
       <c r="X2">
-        <f>M2/W2</f>
+        <f t="shared" ref="X2:X7" si="3">M2/W2</f>
         <v>8.1821311040311817E-3</v>
       </c>
       <c r="Y2">
-        <f>K2^3</f>
+        <f t="shared" ref="Y2:Y7" si="4">K2^3</f>
         <v>512</v>
       </c>
       <c r="Z2">
-        <f>N2/Y2</f>
+        <f t="shared" ref="Z2:Z7" si="5">N2/Y2</f>
         <v>9.8999023437503376E-4</v>
       </c>
     </row>
@@ -8764,7 +8763,7 @@
         <v>5.5450000000001299E-4</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G9" si="0">2^3</f>
+        <f t="shared" ref="G3:G5" si="6">2^3</f>
         <v>8</v>
       </c>
       <c r="H3" s="2">
@@ -8787,43 +8786,43 @@
         <v>2.6863249999999823</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O7" si="1">LOG(K3)</f>
+        <f t="shared" ref="O3:O7" si="7">LOG(K3)</f>
         <v>1.2041199826559248</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P7" si="2">LOG(L3)</f>
+        <f t="shared" ref="P3:P7" si="8">LOG(L3)</f>
         <v>-0.15801519540988565</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q7" si="3">LOG(M3)</f>
+        <f t="shared" ref="Q3:Q7" si="9">LOG(M3)</f>
         <v>1.1270488874539486</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:R7" si="4">LOG(N3)</f>
+        <f t="shared" ref="R3:R7" si="10">LOG(N3)</f>
         <v>0.42915855381599588</v>
       </c>
       <c r="U3">
-        <f>K3^3</f>
+        <f t="shared" si="0"/>
         <v>4096</v>
       </c>
       <c r="V3">
-        <f>L3/U3</f>
+        <f t="shared" si="1"/>
         <v>1.6967773437500018E-4</v>
       </c>
       <c r="W3">
-        <f>K3^2.8</f>
+        <f t="shared" si="2"/>
         <v>2352.5342310339256</v>
       </c>
       <c r="X3">
-        <f>M3/W3</f>
+        <f t="shared" si="3"/>
         <v>5.6952518791241816E-3</v>
       </c>
       <c r="Y3">
-        <f>K3^3</f>
+        <f t="shared" si="4"/>
         <v>4096</v>
       </c>
       <c r="Z3">
-        <f>N3/Y3</f>
+        <f t="shared" si="5"/>
         <v>6.5584106445312068E-4</v>
       </c>
     </row>
@@ -8847,7 +8846,7 @@
         <v>6.1409999999995004E-4</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="H4">
@@ -8870,43 +8869,43 @@
         <v>15.2584249999999</v>
       </c>
       <c r="O4">
+        <f t="shared" si="7"/>
+        <v>1.505149978319906</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="8"/>
+        <v>0.62767047287101851</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="9"/>
+        <v>1.9292943675246235</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="10"/>
+        <v>1.1835097073337799</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="0"/>
+        <v>32768</v>
+      </c>
+      <c r="V4">
         <f t="shared" si="1"/>
-        <v>1.505149978319906</v>
-      </c>
-      <c r="P4">
+        <v>1.2948532104492286E-4</v>
+      </c>
+      <c r="W4">
         <f t="shared" si="2"/>
-        <v>0.62767047287101851</v>
-      </c>
-      <c r="Q4">
+        <v>16383.999999999991</v>
+      </c>
+      <c r="X4">
         <f t="shared" si="3"/>
-        <v>1.9292943675246235</v>
-      </c>
-      <c r="R4">
+        <v>5.1865005493164085E-3</v>
+      </c>
+      <c r="Y4">
         <f t="shared" si="4"/>
-        <v>1.1835097073337799</v>
-      </c>
-      <c r="U4">
-        <f>K4^3</f>
         <v>32768</v>
       </c>
-      <c r="V4">
-        <f>L4/U4</f>
-        <v>1.2948532104492286E-4</v>
-      </c>
-      <c r="W4">
-        <f>K4^2.8</f>
-        <v>16383.999999999991</v>
-      </c>
-      <c r="X4">
-        <f>M4/W4</f>
-        <v>5.1865005493164085E-3</v>
-      </c>
-      <c r="Y4">
-        <f>K4^3</f>
-        <v>32768</v>
-      </c>
       <c r="Z4">
-        <f>N4/Y4</f>
+        <f t="shared" si="5"/>
         <v>4.6565017700195006E-4</v>
       </c>
     </row>
@@ -8930,7 +8929,7 @@
         <v>5.0320000000003695E-4</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="H5">
@@ -8953,43 +8952,43 @@
         <v>97.632549999999995</v>
       </c>
       <c r="O5">
+        <f t="shared" si="7"/>
+        <v>1.8061799739838871</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="8"/>
+        <v>1.4861622386732232</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="9"/>
+        <v>2.7307678662145167</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="10"/>
+        <v>1.9895946325094722</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="0"/>
+        <v>262144</v>
+      </c>
+      <c r="V5">
         <f t="shared" si="1"/>
-        <v>1.8061799739838871</v>
-      </c>
-      <c r="P5">
+        <v>1.1684827804565355E-4</v>
+      </c>
+      <c r="W5">
         <f t="shared" si="2"/>
-        <v>1.4861622386732232</v>
-      </c>
-      <c r="Q5">
+        <v>114104.80343234935</v>
+      </c>
+      <c r="X5">
         <f t="shared" si="3"/>
-        <v>2.7307678662145167</v>
-      </c>
-      <c r="R5">
+        <v>4.7148072107144837E-3</v>
+      </c>
+      <c r="Y5">
         <f t="shared" si="4"/>
-        <v>1.9895946325094722</v>
-      </c>
-      <c r="U5">
-        <f>K5^3</f>
         <v>262144</v>
       </c>
-      <c r="V5">
-        <f>L5/U5</f>
-        <v>1.1684827804565355E-4</v>
-      </c>
-      <c r="W5">
-        <f>K5^2.8</f>
-        <v>114104.80343234935</v>
-      </c>
-      <c r="X5">
-        <f>M5/W5</f>
-        <v>4.7148072107144837E-3</v>
-      </c>
-      <c r="Y5">
-        <f>K5^3</f>
-        <v>262144</v>
-      </c>
       <c r="Z5">
-        <f>N5/Y5</f>
+        <f t="shared" si="5"/>
         <v>3.7243862152099607E-4</v>
       </c>
     </row>
@@ -9039,43 +9038,43 @@
         <v>792.92204999999876</v>
       </c>
       <c r="O6">
+        <f t="shared" si="7"/>
+        <v>2.1072099696478683</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="8"/>
+        <v>2.3777121194114659</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="9"/>
+        <v>3.593352405421244</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="10"/>
+        <v>2.8992304951122811</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="0"/>
+        <v>2097152</v>
+      </c>
+      <c r="V6">
         <f t="shared" si="1"/>
-        <v>2.1072099696478683</v>
-      </c>
-      <c r="P6">
+        <v>1.1378426551818836E-4</v>
+      </c>
+      <c r="W6">
         <f t="shared" si="2"/>
-        <v>2.3777121194114659</v>
-      </c>
-      <c r="Q6">
+        <v>794672.00722260214</v>
+      </c>
+      <c r="X6">
         <f t="shared" si="3"/>
-        <v>3.593352405421244</v>
-      </c>
-      <c r="R6">
+        <v>4.9336063046974375E-3</v>
+      </c>
+      <c r="Y6">
         <f t="shared" si="4"/>
-        <v>2.8992304951122811</v>
-      </c>
-      <c r="U6">
-        <f>K6^3</f>
         <v>2097152</v>
       </c>
-      <c r="V6">
-        <f>L6/U6</f>
-        <v>1.1378426551818836E-4</v>
-      </c>
-      <c r="W6">
-        <f>K6^2.8</f>
-        <v>794672.00722260214</v>
-      </c>
-      <c r="X6">
-        <f>M6/W6</f>
-        <v>4.9336063046974375E-3</v>
-      </c>
-      <c r="Y6">
-        <f>K6^3</f>
-        <v>2097152</v>
-      </c>
       <c r="Z6">
-        <f>N6/Y6</f>
+        <f t="shared" si="5"/>
         <v>3.780946969985956E-4</v>
       </c>
     </row>
@@ -9099,7 +9098,7 @@
         <v>2.3290000000000199E-3</v>
       </c>
       <c r="G7">
-        <f t="shared" ref="G7:G25" si="5">2^4</f>
+        <f t="shared" ref="G7:G9" si="11">2^4</f>
         <v>16</v>
       </c>
       <c r="H7">
@@ -9122,35 +9121,35 @@
         <v>5574.0187000000624</v>
       </c>
       <c r="O7">
+        <f t="shared" si="7"/>
+        <v>2.4082399653118496</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="8"/>
+        <v>3.3689957126871852</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="9"/>
+        <v>4.4929209411274673</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="10"/>
+        <v>3.7461684213728388</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="0"/>
+        <v>16777216</v>
+      </c>
+      <c r="V7">
         <f t="shared" si="1"/>
-        <v>2.4082399653118496</v>
-      </c>
-      <c r="P7">
+        <v>1.3940418660640463E-4</v>
+      </c>
+      <c r="W7">
         <f t="shared" si="2"/>
-        <v>3.3689957126871852</v>
-      </c>
-      <c r="Q7">
+        <v>5534417.3081863848</v>
+      </c>
+      <c r="X7">
         <f t="shared" si="3"/>
-        <v>4.4929209411274673</v>
-      </c>
-      <c r="R7">
-        <f t="shared" si="4"/>
-        <v>3.7461684213728388</v>
-      </c>
-      <c r="U7">
-        <f>K7^3</f>
-        <v>16777216</v>
-      </c>
-      <c r="V7">
-        <f>L7/U7</f>
-        <v>1.3940418660640463E-4</v>
-      </c>
-      <c r="W7">
-        <f>K7^2.8</f>
-        <v>5534417.3081863848</v>
-      </c>
-      <c r="X7">
-        <f>M7/W7</f>
         <v>5.6214588804101521E-3</v>
       </c>
       <c r="Y7">
@@ -9158,7 +9157,7 @@
         <v>16777216</v>
       </c>
       <c r="Z7">
-        <f>N7/Y7</f>
+        <f t="shared" si="5"/>
         <v>3.3223740458488836E-4</v>
       </c>
     </row>
@@ -9182,7 +9181,7 @@
         <v>3.8590000000000499E-3</v>
       </c>
       <c r="G8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>16</v>
       </c>
       <c r="H8">
@@ -9209,7 +9208,7 @@
         <v>2.1526999999998899E-3</v>
       </c>
       <c r="G9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>16</v>
       </c>
       <c r="H9">
@@ -9266,7 +9265,7 @@
         <v>1.4519600000000001E-2</v>
       </c>
       <c r="G11">
-        <f t="shared" ref="G11:G13" si="6">2^5</f>
+        <f t="shared" ref="G11:G13" si="12">2^5</f>
         <v>32</v>
       </c>
       <c r="H11">
@@ -9293,7 +9292,7 @@
         <v>1.5998699999999901E-2</v>
       </c>
       <c r="G12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>32</v>
       </c>
       <c r="H12">
@@ -9320,7 +9319,7 @@
         <v>1.4724799999999901E-2</v>
       </c>
       <c r="G13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>32</v>
       </c>
       <c r="H13">
@@ -9377,7 +9376,7 @@
         <v>9.8696600000000204E-2</v>
       </c>
       <c r="G15">
-        <f t="shared" ref="G15:G17" si="7">2^6</f>
+        <f t="shared" ref="G15:G17" si="13">2^6</f>
         <v>64</v>
       </c>
       <c r="H15">
@@ -9404,7 +9403,7 @@
         <v>9.6874500000000197E-2</v>
       </c>
       <c r="G16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>64</v>
       </c>
       <c r="H16">
@@ -9431,7 +9430,7 @@
         <v>9.60362999999997E-2</v>
       </c>
       <c r="G17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>64</v>
       </c>
       <c r="H17">
@@ -9488,7 +9487,7 @@
         <v>0.95315970000000005</v>
       </c>
       <c r="G19">
-        <f t="shared" ref="G19:G21" si="8">2^7</f>
+        <f t="shared" ref="G19:G21" si="14">2^7</f>
         <v>128</v>
       </c>
       <c r="H19">
@@ -9515,7 +9514,7 @@
         <v>0.70846479999999801</v>
       </c>
       <c r="G20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>128</v>
       </c>
       <c r="H20">
@@ -9542,7 +9541,7 @@
         <v>0.80264559999999796</v>
       </c>
       <c r="G21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>128</v>
       </c>
       <c r="H21">
@@ -9599,7 +9598,7 @@
         <v>5.5329182000000401</v>
       </c>
       <c r="G23">
-        <f t="shared" ref="G23:G25" si="9">2^8</f>
+        <f t="shared" ref="G23:G25" si="15">2^8</f>
         <v>256</v>
       </c>
       <c r="H23">
@@ -9626,7 +9625,7 @@
         <v>5.2064347000000399</v>
       </c>
       <c r="G24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>256</v>
       </c>
       <c r="H24">
@@ -9653,7 +9652,7 @@
         <v>5.4452714000001299</v>
       </c>
       <c r="G25">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>256</v>
       </c>
       <c r="H25">

</xml_diff>